<commit_message>
Added in a few more memory mappings, fixed the EE Core and IOP MMU's to recognise when a read or write is occuring (helps with throwing exceptions and checking for the isolate cache condition).
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Memory Mappings.xlsx
+++ b/PCSX2_Core/Docs/Memory Mappings.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\Dev\Projects\PCSX2_Rewrite\PCSX2_Core\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\Dev\Projects\PCSX2_Rewrite\PCSX2_Core\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>From</t>
   </si>
@@ -35,53 +35,134 @@
     <t>Region/Description</t>
   </si>
   <si>
-    <t>Main Memory</t>
-  </si>
-  <si>
     <t>0x00000000</t>
   </si>
   <si>
     <t>Size (Bytes)</t>
   </si>
   <si>
-    <t>Scratchpad Memory</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>0x14000000</t>
-  </si>
-  <si>
-    <t>PCSX2 PS2 Physical Memory/VM MMU Mappings</t>
-  </si>
-  <si>
-    <t>In general, the mappings are identical and linear between the PS2's physical space and the VM's memory space.</t>
-  </si>
-  <si>
-    <t>Boot ROM</t>
-  </si>
-  <si>
     <t>0x1FC00000</t>
   </si>
   <si>
-    <t>Note 1:</t>
-  </si>
-  <si>
-    <t>Note 2:</t>
-  </si>
-  <si>
-    <t>All memory mappings are established in the VMMain::initalisePS2PhysicalMemory() function.</t>
-  </si>
-  <si>
-    <t>PCSX2 SPECIFIC - does not actually happen on real PS2. However this region where it is allocated ("Reserved") is unused in the emulator, which makes it free to use for mapping. There is no documented PS2 physical address that you can access the scratchpad with.</t>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Size (MB)</t>
+  </si>
+  <si>
+    <t>Size (kB)</t>
+  </si>
+  <si>
+    <t>EE Registers</t>
+  </si>
+  <si>
+    <t>The EE and IOP have separate physical memory space, which is reflected below.</t>
+  </si>
+  <si>
+    <t>EE Mappings</t>
+  </si>
+  <si>
+    <t>0x70000000</t>
+  </si>
+  <si>
+    <t>PCSX2 Rewrite PS2 Physical Memory Mappings</t>
+  </si>
+  <si>
+    <t>0x10000000</t>
+  </si>
+  <si>
+    <t>Hex to Dec Calculator</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>In (without leading 0x)</t>
+  </si>
+  <si>
+    <t>Not officially documented in EE manuals, but the start address seems to pop up a lot using the internet resources. PCSX2 also allocates at this address.</t>
+  </si>
+  <si>
+    <t>GS Registers</t>
+  </si>
+  <si>
+    <t>0x12000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes EE timers, DMAC, etc. See inside the initalisation function for more info. </t>
+  </si>
+  <si>
+    <t>The physical memory map is initalised within the PS2Resources constructor function.</t>
+  </si>
+  <si>
+    <t>Boot ROM1</t>
+  </si>
+  <si>
+    <t>Boot ROM2</t>
+  </si>
+  <si>
+    <t>Boot ROM0</t>
+  </si>
+  <si>
+    <t>0x1E000000</t>
+  </si>
+  <si>
+    <t>0x1E400000</t>
+  </si>
+  <si>
+    <t>EE Core Scratchpad Memory</t>
+  </si>
+  <si>
+    <t>EE Main Memory</t>
+  </si>
+  <si>
+    <t>IOP Main Memory</t>
+  </si>
+  <si>
+    <t>0x1C000000</t>
+  </si>
+  <si>
+    <t>IOP Mappings</t>
+  </si>
+  <si>
+    <t>IOP Registers</t>
+  </si>
+  <si>
+    <t>0x1F800000</t>
+  </si>
+  <si>
+    <t>0x1F801000</t>
+  </si>
+  <si>
+    <t>IOP Core Scratchpad Memory</t>
+  </si>
+  <si>
+    <t>0x1F000000</t>
+  </si>
+  <si>
+    <t>IOP Parallel Port</t>
+  </si>
+  <si>
+    <t>Dec to Hex Calculator</t>
+  </si>
+  <si>
+    <t>Out (without leading 0x)</t>
+  </si>
+  <si>
+    <t>Most of the info gathered from the EE manuals, or PCSX2 otherwise. For the IOP mappings, there are documents online relating to the PSX that have helped.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,8 +185,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,8 +211,13 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -161,20 +255,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
@@ -189,8 +296,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
@@ -284,6 +398,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -319,6 +450,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -471,114 +619,482 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="120.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="27.375" customWidth="1"/>
+    <col min="2" max="2" width="19.75" style="2" customWidth="1"/>
+    <col min="3" max="5" width="22.625" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="120.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <f>HEX2DEC(A8)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" t="str">
+        <f>DEC2HEX(C8)</f>
+        <v>0</v>
+      </c>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="1:7" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    </row>
+    <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5">
+      <c r="C12">
         <f>32*1024*1024</f>
         <v>33554432</v>
       </c>
-      <c r="D5" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B5,8))+C5-1, 8)</f>
+      <c r="D12">
+        <f>C12/1024</f>
+        <v>32768</v>
+      </c>
+      <c r="E12">
+        <f>C12/1024/1024</f>
+        <v>32</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B12,8))+C12-1, 8)</f>
         <v>0x01FFFFFF</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
         <f>16*1024</f>
         <v>16384</v>
       </c>
-      <c r="D6" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B6,8))+C6-1, 8)</f>
-        <v>0x14003FFF</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D13">
+        <f t="shared" ref="D13:D19" si="0">C13/1024</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
+      <c r="E13">
+        <f t="shared" ref="E13:E19" si="1">C13/1024/1024</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="F13" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B13,8))+C13-1, 8)</f>
+        <v>0x70003FFF</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <f>32*1024*1024</f>
+        <v>33554432</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>32768</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B15,8))+C15-1, 8)</f>
+        <v>0x11FFFFFF</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <f>32*1024*1024</f>
+        <v>33554432</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>32768</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="F16" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B16,8))+C16-1, 8)</f>
+        <v>0x13FFFFFF</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2097152</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F18" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B18,8))+C18-1, 8)</f>
+        <v>0x1C1FFFFF</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19">
+        <v>8192</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B19,8))+C19-1, 8)</f>
+        <v>0x1F802FFF</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21">
         <f>4*1024*1024</f>
         <v>4194304</v>
       </c>
-      <c r="D7" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B7,8))+C7-1, 8)</f>
+      <c r="D21">
+        <f>C21/1024</f>
+        <v>4096</v>
+      </c>
+      <c r="E21">
+        <f>C21/1024/1024</f>
+        <v>4</v>
+      </c>
+      <c r="F21" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B21,8))+C21-1, 8)</f>
+        <v>0x1FFFFFFF</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22">
+        <v>262144</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ref="D22:D23" si="2">C22/1024</f>
+        <v>256</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ref="E22:E23" si="3">C22/1024/1024</f>
+        <v>0.25</v>
+      </c>
+      <c r="F22" s="1" t="str">
+        <f t="shared" ref="F22:F23" si="4">"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B22,8))+C22-1, 8)</f>
+        <v>0x1E03FFFF</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23">
+        <v>262144</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>0x1E43FFFF</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:7" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2097152</v>
+      </c>
+      <c r="D27">
+        <f>C27/1024</f>
+        <v>2048</v>
+      </c>
+      <c r="E27">
+        <f>C27/1024/1024</f>
+        <v>2</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B27,8))+C27-1, 8)</f>
+        <v>0x001FFFFF</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29">
+        <v>65536</v>
+      </c>
+      <c r="D29">
+        <f>C29/1024</f>
+        <v>64</v>
+      </c>
+      <c r="E29">
+        <f>C29/1024/1024</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="F29" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B29,8))+C29-1, 8)</f>
+        <v>0x1F00FFFF</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30">
+        <v>1024</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30:D31" si="5">C30/1024</f>
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ref="E30:E31" si="6">C30/1024/1024</f>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="F30" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B30,8))+C30-1, 8)</f>
+        <v>0x1F8003FF</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31">
+        <v>8192</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="6"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="F31" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B31,8))+C31-1, 8)</f>
+        <v>0x1F802FFF</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <f>4*1024*1024</f>
+        <v>4194304</v>
+      </c>
+      <c r="D33">
+        <f>C33/1024</f>
+        <v>4096</v>
+      </c>
+      <c r="E33">
+        <f>C33/1024/1024</f>
+        <v>4</v>
+      </c>
+      <c r="F33" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B33,8))+C33-1, 8)</f>
         <v>0x1FFFFFFF</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Structual changes needed for writing the upcoming VU code. Removed the class / idea of 'bitfield memory 32' and instead changed things to use BitfieldRegister32_t. In order to map a register (into PhysicalMMU_t), a new compatibility layer MappedRegister32_t has been created instead. Any MappedMemory_t class and child classes remain intact, they can still be mapped directly.
</commit_message>
<xml_diff>
--- a/PCSX2_Core/Docs/Memory Mappings.xlsx
+++ b/PCSX2_Core/Docs/Memory Mappings.xlsx
@@ -65,97 +65,97 @@
     <t>EE Mappings</t>
   </si>
   <si>
+    <t>PCSX2 Rewrite PS2 Physical Memory Mappings</t>
+  </si>
+  <si>
+    <t>0x10000000</t>
+  </si>
+  <si>
+    <t>Hex to Dec Calculator</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>In (without leading 0x)</t>
+  </si>
+  <si>
+    <t>GS Registers</t>
+  </si>
+  <si>
+    <t>0x12000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes EE timers, DMAC, etc. See inside the initalisation function for more info. </t>
+  </si>
+  <si>
+    <t>The physical memory map is initalised within the PS2Resources constructor function.</t>
+  </si>
+  <si>
+    <t>Boot ROM1</t>
+  </si>
+  <si>
+    <t>Boot ROM2</t>
+  </si>
+  <si>
+    <t>Boot ROM0</t>
+  </si>
+  <si>
+    <t>0x1E000000</t>
+  </si>
+  <si>
+    <t>0x1E400000</t>
+  </si>
+  <si>
+    <t>EE Core Scratchpad Memory</t>
+  </si>
+  <si>
+    <t>EE Main Memory</t>
+  </si>
+  <si>
+    <t>IOP Main Memory</t>
+  </si>
+  <si>
+    <t>0x1C000000</t>
+  </si>
+  <si>
+    <t>IOP Mappings</t>
+  </si>
+  <si>
+    <t>IOP Registers</t>
+  </si>
+  <si>
+    <t>0x1F800000</t>
+  </si>
+  <si>
+    <t>0x1F801000</t>
+  </si>
+  <si>
+    <t>IOP Core Scratchpad Memory</t>
+  </si>
+  <si>
+    <t>0x1F000000</t>
+  </si>
+  <si>
+    <t>IOP Parallel Port</t>
+  </si>
+  <si>
+    <t>Dec to Hex Calculator</t>
+  </si>
+  <si>
+    <t>Out (without leading 0x)</t>
+  </si>
+  <si>
+    <t>Most of the info gathered from the EE manuals, or PCSX2 otherwise. For the IOP mappings, there are documents online relating to the PSX that have helped.</t>
+  </si>
+  <si>
+    <t>Not officially documented in EE manuals, but the start address seems to pop up a lot using the internet resources. PCSX2 also references this address, although not used through memory maps…</t>
+  </si>
+  <si>
     <t>0x70000000</t>
-  </si>
-  <si>
-    <t>PCSX2 Rewrite PS2 Physical Memory Mappings</t>
-  </si>
-  <si>
-    <t>0x10000000</t>
-  </si>
-  <si>
-    <t>Hex to Dec Calculator</t>
-  </si>
-  <si>
-    <t>In</t>
-  </si>
-  <si>
-    <t>Out</t>
-  </si>
-  <si>
-    <t>In (without leading 0x)</t>
-  </si>
-  <si>
-    <t>Not officially documented in EE manuals, but the start address seems to pop up a lot using the internet resources. PCSX2 also allocates at this address.</t>
-  </si>
-  <si>
-    <t>GS Registers</t>
-  </si>
-  <si>
-    <t>0x12000000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Includes EE timers, DMAC, etc. See inside the initalisation function for more info. </t>
-  </si>
-  <si>
-    <t>The physical memory map is initalised within the PS2Resources constructor function.</t>
-  </si>
-  <si>
-    <t>Boot ROM1</t>
-  </si>
-  <si>
-    <t>Boot ROM2</t>
-  </si>
-  <si>
-    <t>Boot ROM0</t>
-  </si>
-  <si>
-    <t>0x1E000000</t>
-  </si>
-  <si>
-    <t>0x1E400000</t>
-  </si>
-  <si>
-    <t>EE Core Scratchpad Memory</t>
-  </si>
-  <si>
-    <t>EE Main Memory</t>
-  </si>
-  <si>
-    <t>IOP Main Memory</t>
-  </si>
-  <si>
-    <t>0x1C000000</t>
-  </si>
-  <si>
-    <t>IOP Mappings</t>
-  </si>
-  <si>
-    <t>IOP Registers</t>
-  </si>
-  <si>
-    <t>0x1F800000</t>
-  </si>
-  <si>
-    <t>0x1F801000</t>
-  </si>
-  <si>
-    <t>IOP Core Scratchpad Memory</t>
-  </si>
-  <si>
-    <t>0x1F000000</t>
-  </si>
-  <si>
-    <t>IOP Parallel Port</t>
-  </si>
-  <si>
-    <t>Dec to Hex Calculator</t>
-  </si>
-  <si>
-    <t>Out (without leading 0x)</t>
-  </si>
-  <si>
-    <t>Most of the info gathered from the EE manuals, or PCSX2 otherwise. For the IOP mappings, there are documents online relating to the PSX that have helped.</t>
   </si>
 </sst>
 </file>
@@ -619,24 +619,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.375" customWidth="1"/>
-    <col min="2" max="2" width="19.75" style="2" customWidth="1"/>
-    <col min="3" max="5" width="22.625" customWidth="1"/>
-    <col min="6" max="6" width="20.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="120.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="120.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="5"/>
       <c r="F1" s="6"/>
@@ -654,13 +654,13 @@
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F4" s="9"/>
     </row>
@@ -670,26 +670,26 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G7"/>
     </row>
@@ -737,7 +737,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>3</v>
@@ -759,39 +759,39 @@
         <v>0x01FFFFFF</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <f>16*1024</f>
-        <v>16384</v>
-      </c>
-      <c r="D13">
-        <f t="shared" ref="D13:D19" si="0">C13/1024</f>
-        <v>16</v>
-      </c>
-      <c r="E13">
-        <f t="shared" ref="E13:E19" si="1">C13/1024/1024</f>
-        <v>1.5625E-2</v>
-      </c>
-      <c r="F13" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B13,8))+C13-1, 8)</f>
-        <v>0x70003FFF</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>20</v>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <f>32*1024*1024</f>
+        <v>33554432</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D18" si="0">C14/1024</f>
+        <v>32768</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14:E18" si="1">C14/1024/1024</f>
+        <v>32</v>
+      </c>
+      <c r="F14" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B14,8))+C14-1, 8)</f>
+        <v>0x11FFFFFF</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <f>32*1024*1024</f>
@@ -807,225 +807,202 @@
       </c>
       <c r="F15" s="1" t="str">
         <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B15,8))+C15-1, 8)</f>
-        <v>0x11FFFFFF</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16">
-        <f>32*1024*1024</f>
-        <v>33554432</v>
-      </c>
-      <c r="D16">
+        <v>0x13FFFFFF</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2097152</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="0"/>
-        <v>32768</v>
-      </c>
-      <c r="E16">
+        <v>2048</v>
+      </c>
+      <c r="E17">
         <f t="shared" si="1"/>
-        <v>32</v>
-      </c>
-      <c r="F16" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B16,8))+C16-1, 8)</f>
-        <v>0x13FFFFFF</v>
+        <v>2</v>
+      </c>
+      <c r="F17" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B17,8))+C17-1, 8)</f>
+        <v>0x1C1FFFFF</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="1">
-        <v>2097152</v>
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>8192</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>2048</v>
+        <v>8</v>
       </c>
       <c r="E18">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>7.8125E-3</v>
       </c>
       <c r="F18" s="1" t="str">
         <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B18,8))+C18-1, 8)</f>
-        <v>0x1C1FFFFF</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19">
-        <v>8192</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>7.8125E-3</v>
-      </c>
-      <c r="F19" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B19,8))+C19-1, 8)</f>
         <v>0x1F802FFF</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <f>4*1024*1024</f>
+        <v>4194304</v>
+      </c>
+      <c r="D20">
+        <f>C20/1024</f>
+        <v>4096</v>
+      </c>
+      <c r="E20">
+        <f>C20/1024/1024</f>
+        <v>4</v>
+      </c>
+      <c r="F20" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B20,8))+C20-1, 8)</f>
+        <v>0x1FFFFFFF</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C21">
-        <f>4*1024*1024</f>
-        <v>4194304</v>
+        <v>262144</v>
       </c>
       <c r="D21">
-        <f>C21/1024</f>
-        <v>4096</v>
+        <f t="shared" ref="D21:D22" si="2">C21/1024</f>
+        <v>256</v>
       </c>
       <c r="E21">
-        <f>C21/1024/1024</f>
-        <v>4</v>
+        <f t="shared" ref="E21:E22" si="3">C21/1024/1024</f>
+        <v>0.25</v>
       </c>
       <c r="F21" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B21,8))+C21-1, 8)</f>
-        <v>0x1FFFFFFF</v>
+        <f t="shared" ref="F21:F22" si="4">"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B21,8))+C21-1, 8)</f>
+        <v>0x1E03FFFF</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>262144</v>
       </c>
       <c r="D22">
-        <f t="shared" ref="D22:D23" si="2">C22/1024</f>
-        <v>256</v>
-      </c>
-      <c r="E22">
-        <f t="shared" ref="E22:E23" si="3">C22/1024/1024</f>
-        <v>0.25</v>
-      </c>
-      <c r="F22" s="1" t="str">
-        <f t="shared" ref="F22:F23" si="4">"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B22,8))+C22-1, 8)</f>
-        <v>0x1E03FFFF</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23">
-        <v>262144</v>
-      </c>
-      <c r="D23">
         <f t="shared" si="2"/>
         <v>256</v>
       </c>
-      <c r="E23">
+      <c r="E22">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="F23" s="1" t="str">
+      <c r="F22" s="1" t="str">
         <f t="shared" si="4"/>
         <v>0x1E43FFFF</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:7" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24">
+        <f>16*1024</f>
+        <v>16384</v>
+      </c>
+      <c r="D24">
+        <f>C24/1024</f>
+        <v>16</v>
+      </c>
+      <c r="E24">
+        <f>C24/1024/1024</f>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="F24" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B24,8))+C24-1, 8)</f>
+        <v>0x70003FFF</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:7" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="12" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B27" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D27" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E27" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F27" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G27" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="28" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C28" s="1">
         <v>2097152</v>
       </c>
-      <c r="D27">
-        <f>C27/1024</f>
+      <c r="D28">
+        <f>C28/1024</f>
         <v>2048</v>
       </c>
-      <c r="E27">
-        <f>C27/1024/1024</f>
+      <c r="E28">
+        <f>C28/1024/1024</f>
         <v>2</v>
       </c>
-      <c r="F27" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B27,8))+C27-1, 8)</f>
+      <c r="F28" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B28,8))+C28-1, 8)</f>
         <v>0x001FFFFF</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29">
-        <v>65536</v>
-      </c>
-      <c r="D29">
-        <f>C29/1024</f>
-        <v>64</v>
-      </c>
-      <c r="E29">
-        <f>C29/1024/1024</f>
-        <v>6.25E-2</v>
-      </c>
-      <c r="F29" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B29,8))+C29-1, 8)</f>
-        <v>0x1F00FFFF</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1033,68 +1010,91 @@
         <v>38</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C30">
-        <v>1024</v>
+        <v>65536</v>
       </c>
       <c r="D30">
-        <f t="shared" ref="D30:D31" si="5">C30/1024</f>
-        <v>1</v>
+        <f>C30/1024</f>
+        <v>64</v>
       </c>
       <c r="E30">
-        <f t="shared" ref="E30:E31" si="6">C30/1024/1024</f>
-        <v>9.765625E-4</v>
+        <f>C30/1024/1024</f>
+        <v>6.25E-2</v>
       </c>
       <c r="F30" s="1" t="str">
         <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B30,8))+C30-1, 8)</f>
-        <v>0x1F8003FF</v>
+        <v>0x1F00FFFF</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>1024</v>
+      </c>
+      <c r="D31">
+        <f t="shared" ref="D31:D32" si="5">C31/1024</f>
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <f t="shared" ref="E31:E32" si="6">C31/1024/1024</f>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="F31" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B31,8))+C31-1, 8)</f>
+        <v>0x1F8003FF</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31">
+      <c r="C32">
         <v>8192</v>
       </c>
-      <c r="D31">
+      <c r="D32">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="E31">
+      <c r="E32">
         <f t="shared" si="6"/>
         <v>7.8125E-3</v>
       </c>
-      <c r="F31" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B31,8))+C31-1, 8)</f>
+      <c r="F32" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B32,8))+C32-1, 8)</f>
         <v>0x1F802FFF</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="2" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C33">
+      <c r="C34">
         <f>4*1024*1024</f>
         <v>4194304</v>
       </c>
-      <c r="D33">
-        <f>C33/1024</f>
+      <c r="D34">
+        <f>C34/1024</f>
         <v>4096</v>
       </c>
-      <c r="E33">
-        <f>C33/1024/1024</f>
+      <c r="E34">
+        <f>C34/1024/1024</f>
         <v>4</v>
       </c>
-      <c r="F33" s="1" t="str">
-        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B33,8))+C33-1, 8)</f>
+      <c r="F34" s="1" t="str">
+        <f>"0x"&amp;DEC2HEX(HEX2DEC(RIGHT(B34,8))+C34-1, 8)</f>
         <v>0x1FFFFFFF</v>
       </c>
     </row>

</xml_diff>